<commit_message>
fixed UI with logo and plot, dont know why it broke last time
</commit_message>
<xml_diff>
--- a/Test_A.xlsx
+++ b/Test_A.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="3">
   <si>
     <t>Var1</t>
   </si>
@@ -44,7 +44,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="89">
     <border>
       <left/>
       <right/>
@@ -84,11 +84,67 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -122,6 +178,62 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="44" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="48" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="52" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="53" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="54" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="55" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="56" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="57" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="58" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="59" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="60" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="61" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="62" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="63" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="64" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="65" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="66" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="67" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="68" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="69" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="70" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="71" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="72" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="73" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="74" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="75" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="76" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="77" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="78" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="79" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="80" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="81" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="82" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="83" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="84" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="85" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="86" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="87" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="88" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -140,25 +252,25 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="29" t="s">
+      <c r="A1" s="85" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="85" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2">
       <c r="A2">
-        <v>76.920000000000002</v>
+        <v>-89.010000000000005</v>
       </c>
       <c r="B2">
-        <v>0.17999999999999999</v>
+        <v>12.970000000000001</v>
       </c>
       <c r="C2">
-        <v>-80.069999999999993</v>
+        <v>109.52</v>
       </c>
     </row>
   </sheetData>
@@ -170,520 +282,523 @@
   <dimension ref="A1:C330"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="true"/>
+    <col min="1" max="1" width="5.7109375" customWidth="true"/>
     <col min="2" max="2" width="4.7109375" customWidth="true"/>
     <col min="3" max="3" width="4.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="31" t="s">
+      <c r="A1" s="87" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="87" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2">
       <c r="A2">
-        <v>605</v>
+        <v>303</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="C2">
-        <v>-1</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>705</v>
+        <v>403</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="C3">
-        <v>-1</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>806</v>
+        <v>505</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="C4">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>907</v>
+        <v>605</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="C5">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>1007</v>
+        <v>707</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>0.10000000000000001</v>
       </c>
       <c r="C6">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
+        <v>1009</v>
+      </c>
+      <c r="B7">
+        <v>0.13</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
         <v>1109</v>
       </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="8">
       <c r="B8">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="C8">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>1310</v>
+        <v>1210</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="C9">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>1411</v>
+        <v>1311</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="C10">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>1512</v>
+        <v>1412</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="C11">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>1613</v>
+        <v>1512</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="C12">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>1714</v>
+        <v>1614</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="C13">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>1814</v>
+        <v>1714</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="C14">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>1916</v>
+        <v>1816</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="C15">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>2016</v>
+        <v>1916</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="C16">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>2135</v>
+        <v>2017</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="C17">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>2236</v>
+        <v>2136</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="C18">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>2337</v>
+        <v>2237</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="C19">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>2438</v>
+        <v>2338</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="C20">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>2538</v>
+        <v>2439</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>0.14999999999999999</v>
       </c>
       <c r="C21">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>2640</v>
+        <v>2540</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>0.14999999999999999</v>
       </c>
       <c r="C22">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>2740</v>
+        <v>2641</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="C23">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>2841</v>
+        <v>2741</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="C24">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>2942</v>
+        <v>2843</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="C25">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>3042</v>
+        <v>2943</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="C26">
-        <v>-1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>3143</v>
+        <v>3044</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>0.17000000000000001</v>
       </c>
       <c r="C27">
-        <v>-1</v>
+        <v>254</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>3244</v>
+        <v>3145</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>0.17999999999999999</v>
       </c>
       <c r="C28">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>3345</v>
+        <v>3246</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>0.19</v>
       </c>
       <c r="C29">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>3446</v>
+        <v>3346</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>0.19</v>
       </c>
       <c r="C30">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>3547</v>
+        <v>3448</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>0.19</v>
       </c>
       <c r="C31">
-        <v>-1</v>
+        <v>252</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>3647</v>
+        <v>3548</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>0.17999999999999999</v>
       </c>
       <c r="C32">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>3749</v>
+        <v>3650</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>0.19</v>
       </c>
       <c r="C33">
-        <v>-1</v>
+        <v>255</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
-        <v>3849</v>
+        <v>3750</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>0.17999999999999999</v>
       </c>
       <c r="C34">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35">
-        <v>3950</v>
+        <v>3851</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>0.17000000000000001</v>
       </c>
       <c r="C35">
-        <v>-1</v>
+        <v>255</v>
       </c>
     </row>
     <row r="36">
       <c r="A36">
-        <v>4051</v>
+        <v>3952</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>0.17000000000000001</v>
       </c>
       <c r="C36">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
       <c r="A37">
-        <v>4170</v>
+        <v>4053</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>0.17999999999999999</v>
       </c>
       <c r="C37">
-        <v>-1</v>
+        <v>192</v>
       </c>
     </row>
     <row r="38">
       <c r="A38">
-        <v>4271</v>
+        <v>4172</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="C38">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
       <c r="A39">
-        <v>4371</v>
+        <v>4273</v>
       </c>
       <c r="B39">
-        <v>0</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="C39">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40">
-        <v>4473</v>
+        <v>4374</v>
       </c>
       <c r="B40">
-        <v>0</v>
+        <v>0.29999999999999999</v>
       </c>
       <c r="C40">
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41">
       <c r="A41">
-        <v>4573</v>
+        <v>4475</v>
       </c>
       <c r="B41">
-        <v>0</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="C41">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42">
-        <v>4674</v>
+        <v>4576</v>
       </c>
       <c r="B42">
-        <v>0</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="C42">
-        <v>-1</v>
+        <v>254</v>
       </c>
     </row>
     <row r="43">
       <c r="A43">
-        <v>4775</v>
+        <v>4677</v>
       </c>
       <c r="B43">
-        <v>0</v>
+        <v>0.29999999999999999</v>
       </c>
       <c r="C43">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44">
-        <v>4876</v>
+        <v>4778</v>
       </c>
       <c r="B44">
-        <v>0</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="C44">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45">
-        <v>4976</v>
+        <v>4878</v>
       </c>
       <c r="B45">
-        <v>0</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="C45">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46">
-        <v>5078</v>
+        <v>4980</v>
       </c>
       <c r="B46">
-        <v>0</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="C46">
-        <v>-1</v>
+        <v>241</v>
       </c>
     </row>
     <row r="47">
       <c r="A47">
-        <v>5882</v>
+        <v>5080</v>
       </c>
       <c r="B47">
-        <v>0</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -691,21 +806,21 @@
     </row>
     <row r="48">
       <c r="A48">
-        <v>5983</v>
+        <v>5181</v>
       </c>
       <c r="B48">
-        <v>0</v>
+        <v>0.27000000000000002</v>
       </c>
       <c r="C48">
-        <v>0</v>
+        <v>255</v>
       </c>
     </row>
     <row r="49">
       <c r="A49">
-        <v>6084</v>
+        <v>5282</v>
       </c>
       <c r="B49">
-        <v>0</v>
+        <v>0.27000000000000002</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -713,10 +828,10 @@
     </row>
     <row r="50">
       <c r="A50">
-        <v>6203</v>
+        <v>5383</v>
       </c>
       <c r="B50">
-        <v>0</v>
+        <v>0.27000000000000002</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -724,21 +839,21 @@
     </row>
     <row r="51">
       <c r="A51">
-        <v>6303</v>
+        <v>5484</v>
       </c>
       <c r="B51">
-        <v>0</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="C51">
-        <v>0</v>
+        <v>248</v>
       </c>
     </row>
     <row r="52">
       <c r="A52">
-        <v>6404</v>
+        <v>5585</v>
       </c>
       <c r="B52">
-        <v>0</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -746,10 +861,10 @@
     </row>
     <row r="53">
       <c r="A53">
-        <v>6505</v>
+        <v>5685</v>
       </c>
       <c r="B53">
-        <v>0</v>
+        <v>0.27000000000000002</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -757,10 +872,10 @@
     </row>
     <row r="54">
       <c r="A54">
-        <v>6606</v>
+        <v>5787</v>
       </c>
       <c r="B54">
-        <v>0</v>
+        <v>0.27000000000000002</v>
       </c>
       <c r="C54">
         <v>0</v>
@@ -768,10 +883,10 @@
     </row>
     <row r="55">
       <c r="A55">
-        <v>6707</v>
+        <v>5887</v>
       </c>
       <c r="B55">
-        <v>0</v>
+        <v>0.26000000000000001</v>
       </c>
       <c r="C55">
         <v>0</v>
@@ -779,21 +894,21 @@
     </row>
     <row r="56">
       <c r="A56">
-        <v>6807</v>
+        <v>5988</v>
       </c>
       <c r="B56">
-        <v>0</v>
+        <v>0.27000000000000002</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>254</v>
       </c>
     </row>
     <row r="57">
       <c r="A57">
-        <v>6908</v>
+        <v>6089</v>
       </c>
       <c r="B57">
-        <v>0</v>
+        <v>0.23999999999999999</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -801,1616 +916,1616 @@
     </row>
     <row r="58">
       <c r="A58">
-        <v>7009</v>
+        <v>6209</v>
       </c>
       <c r="B58">
-        <v>0</v>
+        <v>0.40000000000000002</v>
       </c>
       <c r="C58">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59">
       <c r="A59">
-        <v>6715</v>
+        <v>6309</v>
       </c>
       <c r="B59">
-        <v>0.91000000000000003</v>
+        <v>0.39000000000000001</v>
       </c>
       <c r="C59">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60">
       <c r="A60">
-        <v>6816</v>
+        <v>6410</v>
       </c>
       <c r="B60">
-        <v>0.93999999999999995</v>
+        <v>0.38</v>
       </c>
       <c r="C60">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="61">
       <c r="A61">
-        <v>6916</v>
+        <v>6511</v>
       </c>
       <c r="B61">
-        <v>0.93999999999999995</v>
+        <v>0.39000000000000001</v>
       </c>
       <c r="C61">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="62">
       <c r="A62">
-        <v>7018</v>
+        <v>6612</v>
       </c>
       <c r="B62">
-        <v>0.81999999999999995</v>
+        <v>0.35999999999999999</v>
       </c>
       <c r="C62">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="63">
       <c r="A63">
-        <v>7118</v>
+        <v>6712</v>
       </c>
       <c r="B63">
-        <v>0.79000000000000004</v>
+        <v>0.38</v>
       </c>
       <c r="C63">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="64">
       <c r="A64">
-        <v>7219</v>
+        <v>6814</v>
       </c>
       <c r="B64">
-        <v>0.82999999999999996</v>
+        <v>0.39000000000000001</v>
       </c>
       <c r="C64">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="65">
       <c r="A65">
-        <v>7320</v>
+        <v>6914</v>
       </c>
       <c r="B65">
-        <v>0.85999999999999999</v>
+        <v>0.34999999999999998</v>
       </c>
       <c r="C65">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="66">
       <c r="A66">
-        <v>7421</v>
+        <v>7015</v>
       </c>
       <c r="B66">
-        <v>0.82999999999999996</v>
+        <v>0.38</v>
       </c>
       <c r="C66">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="67">
       <c r="A67">
-        <v>7521</v>
+        <v>7116</v>
       </c>
       <c r="B67">
-        <v>0.77000000000000002</v>
+        <v>0.35999999999999999</v>
       </c>
       <c r="C67">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="68">
       <c r="A68">
-        <v>7623</v>
+        <v>7217</v>
       </c>
       <c r="B68">
-        <v>0.71999999999999997</v>
+        <v>0.37</v>
       </c>
       <c r="C68">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="69">
       <c r="A69">
-        <v>7723</v>
+        <v>7319</v>
       </c>
       <c r="B69">
-        <v>0.69999999999999996</v>
+        <v>0.35999999999999999</v>
       </c>
       <c r="C69">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="70">
       <c r="A70">
-        <v>7825</v>
+        <v>7419</v>
       </c>
       <c r="B70">
-        <v>0.71999999999999997</v>
+        <v>0.35999999999999999</v>
       </c>
       <c r="C70">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="71">
       <c r="A71">
-        <v>7926</v>
+        <v>7520</v>
       </c>
       <c r="B71">
-        <v>0.71999999999999997</v>
+        <v>0.35999999999999999</v>
       </c>
       <c r="C71">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="72">
       <c r="A72">
-        <v>8026</v>
+        <v>7621</v>
       </c>
       <c r="B72">
-        <v>0.78000000000000003</v>
+        <v>0.34999999999999998</v>
       </c>
       <c r="C72">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="73">
       <c r="A73">
-        <v>8128</v>
+        <v>7722</v>
       </c>
       <c r="B73">
-        <v>0.78000000000000003</v>
+        <v>0.35999999999999999</v>
       </c>
       <c r="C73">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="74">
       <c r="A74">
-        <v>8246</v>
+        <v>7822</v>
       </c>
       <c r="B74">
-        <v>1.1499999999999999</v>
+        <v>0.34999999999999998</v>
       </c>
       <c r="C74">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="75">
       <c r="A75">
-        <v>8348</v>
+        <v>7924</v>
       </c>
       <c r="B75">
-        <v>1.0800000000000001</v>
+        <v>0.34999999999999998</v>
       </c>
       <c r="C75">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="76">
       <c r="A76">
-        <v>8448</v>
+        <v>8024</v>
       </c>
       <c r="B76">
-        <v>1.02</v>
+        <v>0.35999999999999999</v>
       </c>
       <c r="C76">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="77">
       <c r="A77">
-        <v>8550</v>
+        <v>8125</v>
       </c>
       <c r="B77">
-        <v>1.0900000000000001</v>
+        <v>0.34999999999999998</v>
       </c>
       <c r="C77">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="78">
       <c r="A78">
-        <v>8650</v>
+        <v>8244</v>
       </c>
       <c r="B78">
-        <v>1.1200000000000001</v>
+        <v>0.54000000000000004</v>
       </c>
       <c r="C78">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="79">
       <c r="A79">
-        <v>8751</v>
+        <v>8346</v>
       </c>
       <c r="B79">
-        <v>1.0900000000000001</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C79">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="80">
       <c r="A80">
-        <v>8852</v>
+        <v>8446</v>
       </c>
       <c r="B80">
-        <v>1.1000000000000001</v>
+        <v>0.63</v>
       </c>
       <c r="C80">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="81">
       <c r="A81">
-        <v>8953</v>
+        <v>8547</v>
       </c>
       <c r="B81">
-        <v>1.1100000000000001</v>
+        <v>0.62</v>
       </c>
       <c r="C81">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="82">
       <c r="A82">
-        <v>9053</v>
+        <v>8648</v>
       </c>
       <c r="B82">
-        <v>1.1200000000000001</v>
+        <v>0.59999999999999998</v>
       </c>
       <c r="C82">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="83">
       <c r="A83">
-        <v>9155</v>
+        <v>8749</v>
       </c>
       <c r="B83">
-        <v>1.0900000000000001</v>
+        <v>0.59999999999999998</v>
       </c>
       <c r="C83">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="84">
       <c r="A84">
-        <v>9255</v>
+        <v>8850</v>
       </c>
       <c r="B84">
-        <v>1.0900000000000001</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="C84">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="85">
       <c r="A85">
-        <v>9356</v>
+        <v>8951</v>
       </c>
       <c r="B85">
-        <v>1.0900000000000001</v>
+        <v>0.53000000000000003</v>
       </c>
       <c r="C85">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="86">
       <c r="A86">
-        <v>9457</v>
+        <v>9052</v>
       </c>
       <c r="B86">
-        <v>1.0900000000000001</v>
+        <v>0.58999999999999997</v>
       </c>
       <c r="C86">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="87">
       <c r="A87">
-        <v>9558</v>
+        <v>9153</v>
       </c>
       <c r="B87">
-        <v>1.0900000000000001</v>
+        <v>0.58999999999999997</v>
       </c>
       <c r="C87">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="88">
       <c r="A88">
-        <v>9659</v>
+        <v>9254</v>
       </c>
       <c r="B88">
-        <v>1.0900000000000001</v>
+        <v>0.58999999999999997</v>
       </c>
       <c r="C88">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="89">
       <c r="A89">
-        <v>9760</v>
+        <v>9354</v>
       </c>
       <c r="B89">
-        <v>1.0600000000000001</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="C89">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="90">
       <c r="A90">
-        <v>9860</v>
+        <v>9456</v>
       </c>
       <c r="B90">
-        <v>1.1200000000000001</v>
+        <v>0.58999999999999997</v>
       </c>
       <c r="C90">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="91">
       <c r="A91">
-        <v>9962</v>
+        <v>9556</v>
       </c>
       <c r="B91">
-        <v>1.21</v>
+        <v>0.62</v>
       </c>
       <c r="C91">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="92">
       <c r="A92">
-        <v>10063</v>
+        <v>9657</v>
       </c>
       <c r="B92">
-        <v>1.27</v>
+        <v>0.59999999999999998</v>
       </c>
       <c r="C92">
-        <v>-1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="93">
       <c r="A93">
-        <v>10163</v>
+        <v>9759</v>
       </c>
       <c r="B93">
-        <v>1.27</v>
+        <v>0.60999999999999999</v>
       </c>
       <c r="C93">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="94">
       <c r="A94">
-        <v>10283</v>
+        <v>9859</v>
       </c>
       <c r="B94">
-        <v>1.51</v>
+        <v>0.63</v>
       </c>
       <c r="C94">
-        <v>-1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="95">
       <c r="A95">
-        <v>10384</v>
+        <v>9960</v>
       </c>
       <c r="B95">
-        <v>1.4199999999999999</v>
+        <v>0.63</v>
       </c>
       <c r="C95">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="96">
       <c r="A96">
-        <v>10485</v>
+        <v>10061</v>
       </c>
       <c r="B96">
-        <v>1.3700000000000001</v>
+        <v>0.63</v>
       </c>
       <c r="C96">
-        <v>-1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="97">
       <c r="A97">
-        <v>10585</v>
+        <v>10162</v>
       </c>
       <c r="B97">
-        <v>1.3100000000000001</v>
+        <v>0.67000000000000004</v>
       </c>
       <c r="C97">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="98">
       <c r="A98">
-        <v>10687</v>
+        <v>10281</v>
       </c>
       <c r="B98">
-        <v>1.1499999999999999</v>
+        <v>0.88</v>
       </c>
       <c r="C98">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="99">
       <c r="A99">
-        <v>10787</v>
+        <v>10382</v>
       </c>
       <c r="B99">
-        <v>1.1699999999999999</v>
+        <v>0.89000000000000001</v>
       </c>
       <c r="C99">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="100">
       <c r="A100">
-        <v>10888</v>
+        <v>10483</v>
       </c>
       <c r="B100">
-        <v>1.0600000000000001</v>
+        <v>0.93999999999999995</v>
       </c>
       <c r="C100">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="101">
       <c r="A101">
-        <v>10989</v>
+        <v>10584</v>
       </c>
       <c r="B101">
-        <v>1.01</v>
+        <v>0.98999999999999999</v>
       </c>
       <c r="C101">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="102">
       <c r="A102">
-        <v>11090</v>
+        <v>10685</v>
       </c>
       <c r="B102">
-        <v>1</v>
+        <v>0.94999999999999996</v>
       </c>
       <c r="C102">
-        <v>-1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="103">
       <c r="A103">
-        <v>11191</v>
+        <v>10786</v>
       </c>
       <c r="B103">
-        <v>1.0700000000000001</v>
+        <v>0.93999999999999995</v>
       </c>
       <c r="C103">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="104">
       <c r="A104">
-        <v>11292</v>
+        <v>10887</v>
       </c>
       <c r="B104">
-        <v>1.1200000000000001</v>
+        <v>0.93999999999999995</v>
       </c>
       <c r="C104">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="105">
-      <c r="A105">
-        <v>11393</v>
-      </c>
       <c r="B105">
-        <v>1.05</v>
+        <v>0.93000000000000005</v>
       </c>
       <c r="C105">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="106">
       <c r="A106">
-        <v>11494</v>
+        <v>11190</v>
       </c>
       <c r="B106">
-        <v>1.1399999999999999</v>
+        <v>0.90000000000000002</v>
       </c>
       <c r="C106">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="107">
       <c r="A107">
-        <v>11595</v>
+        <v>11291</v>
       </c>
       <c r="B107">
-        <v>1.05</v>
+        <v>0.91000000000000003</v>
       </c>
       <c r="C107">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="108">
       <c r="A108">
-        <v>11695</v>
+        <v>11594</v>
       </c>
       <c r="B108">
-        <v>1.02</v>
+        <v>0.93000000000000005</v>
       </c>
       <c r="C108">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="109">
       <c r="A109">
-        <v>11797</v>
+        <v>11694</v>
       </c>
       <c r="B109">
-        <v>1.0900000000000001</v>
+        <v>0.93000000000000005</v>
       </c>
       <c r="C109">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="110">
       <c r="A110">
-        <v>11898</v>
+        <v>11795</v>
       </c>
       <c r="B110">
-        <v>1.22</v>
+        <v>0.93000000000000005</v>
       </c>
       <c r="C110">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="111">
       <c r="A111">
-        <v>11998</v>
+        <v>12099</v>
       </c>
       <c r="B111">
-        <v>1.29</v>
+        <v>0.95999999999999996</v>
       </c>
       <c r="C111">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="112">
       <c r="A112">
-        <v>12100</v>
+        <v>12199</v>
       </c>
       <c r="B112">
-        <v>1.27</v>
+        <v>0.95999999999999996</v>
       </c>
       <c r="C112">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="113">
       <c r="A113">
-        <v>12200</v>
+        <v>12319</v>
       </c>
       <c r="B113">
-        <v>1.28</v>
+        <v>1.3600000000000001</v>
       </c>
       <c r="C113">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="114">
       <c r="A114">
-        <v>12320</v>
+        <v>12419</v>
       </c>
       <c r="B114">
         <v>1.3</v>
       </c>
       <c r="C114">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="115">
       <c r="A115">
-        <v>12420</v>
+        <v>2520</v>
       </c>
       <c r="B115">
-        <v>1.2</v>
+        <v>1.3700000000000001</v>
       </c>
       <c r="C115">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="116">
       <c r="A116">
-        <v>12522</v>
+        <v>12722</v>
       </c>
       <c r="B116">
-        <v>1.1399999999999999</v>
+        <v>1.3</v>
       </c>
       <c r="C116">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="117">
       <c r="A117">
-        <v>12622</v>
+        <v>12824</v>
       </c>
       <c r="B117">
-        <v>1.1599999999999999</v>
+        <v>1.25</v>
       </c>
       <c r="C117">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="118">
       <c r="A118">
-        <v>12723</v>
+        <v>12924</v>
       </c>
       <c r="B118">
-        <v>1.1899999999999999</v>
+        <v>1.27</v>
       </c>
       <c r="C118">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="119">
       <c r="A119">
-        <v>12825</v>
+        <v>13025</v>
       </c>
       <c r="B119">
-        <v>1.1499999999999999</v>
+        <v>1.27</v>
       </c>
       <c r="C119">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="120">
       <c r="A120">
-        <v>12925</v>
+        <v>13126</v>
       </c>
       <c r="B120">
-        <v>1</v>
+        <v>1.26</v>
       </c>
       <c r="C120">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="121">
       <c r="A121">
-        <v>13026</v>
+        <v>13227</v>
       </c>
       <c r="B121">
-        <v>1.0900000000000001</v>
+        <v>1.22</v>
       </c>
       <c r="C121">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="122">
       <c r="A122">
-        <v>13127</v>
+        <v>13328</v>
       </c>
       <c r="B122">
-        <v>1.1699999999999999</v>
+        <v>1.21</v>
       </c>
       <c r="C122">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="123">
       <c r="A123">
-        <v>13228</v>
+        <v>13429</v>
       </c>
       <c r="B123">
-        <v>1.0600000000000001</v>
+        <v>1.21</v>
       </c>
       <c r="C123">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="124">
       <c r="A124">
-        <v>13329</v>
+        <v>13530</v>
       </c>
       <c r="B124">
-        <v>0.87</v>
+        <v>1.2</v>
       </c>
       <c r="C124">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="125">
       <c r="A125">
-        <v>13430</v>
+        <v>13630</v>
       </c>
       <c r="B125">
-        <v>1.0900000000000001</v>
+        <v>1.1799999999999999</v>
       </c>
       <c r="C125">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="126">
       <c r="A126">
-        <v>13530</v>
+        <v>13732</v>
       </c>
       <c r="B126">
-        <v>1.0700000000000001</v>
+        <v>1.1699999999999999</v>
       </c>
       <c r="C126">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="127">
       <c r="A127">
-        <v>13632</v>
+        <v>13832</v>
       </c>
       <c r="B127">
-        <v>1.01</v>
+        <v>1.1899999999999999</v>
       </c>
       <c r="C127">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="128">
       <c r="A128">
-        <v>13733</v>
+        <v>13934</v>
       </c>
       <c r="B128">
-        <v>0.98999999999999999</v>
+        <v>1.1799999999999999</v>
       </c>
       <c r="C128">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="129">
       <c r="A129">
-        <v>13833</v>
+        <v>14035</v>
       </c>
       <c r="B129">
-        <v>0.93000000000000005</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="C129">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="130">
       <c r="A130">
-        <v>13935</v>
+        <v>14135</v>
       </c>
       <c r="B130">
-        <v>0.90000000000000002</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="C130">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="131">
       <c r="A131">
-        <v>14035</v>
+        <v>14237</v>
       </c>
       <c r="B131">
-        <v>0.93999999999999995</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="C131">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="132">
       <c r="A132">
-        <v>14136</v>
+        <v>14355</v>
       </c>
       <c r="B132">
-        <v>1.1200000000000001</v>
+        <v>1.6299999999999999</v>
       </c>
       <c r="C132">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="133">
       <c r="A133">
-        <v>14237</v>
+        <v>14457</v>
       </c>
       <c r="B133">
-        <v>1.25</v>
+        <v>1.6799999999999999</v>
       </c>
       <c r="C133">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="134">
       <c r="A134">
-        <v>14357</v>
+        <v>14558</v>
       </c>
       <c r="B134">
-        <v>1.49</v>
+        <v>1.77</v>
       </c>
       <c r="C134">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="135">
       <c r="A135">
-        <v>14457</v>
+        <v>14659</v>
       </c>
       <c r="B135">
-        <v>1.49</v>
+        <v>1.73</v>
       </c>
       <c r="C135">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="136">
       <c r="A136">
-        <v>14558</v>
+        <v>14760</v>
       </c>
       <c r="B136">
-        <v>1.3</v>
+        <v>1.71</v>
       </c>
       <c r="C136">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="137">
       <c r="A137">
-        <v>14660</v>
+        <v>14860</v>
       </c>
       <c r="B137">
-        <v>1.1499999999999999</v>
+        <v>1.6799999999999999</v>
       </c>
       <c r="C137">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="138">
       <c r="A138">
-        <v>14760</v>
+        <v>14962</v>
       </c>
       <c r="B138">
-        <v>1.22</v>
+        <v>1.6699999999999999</v>
       </c>
       <c r="C138">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="139">
       <c r="A139">
-        <v>14861</v>
+        <v>15062</v>
       </c>
       <c r="B139">
-        <v>1.3600000000000001</v>
+        <v>1.6799999999999999</v>
       </c>
       <c r="C139">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="140">
       <c r="A140">
-        <v>14962</v>
+        <v>15163</v>
       </c>
       <c r="B140">
-        <v>1.3100000000000001</v>
+        <v>1.6299999999999999</v>
       </c>
       <c r="C140">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="141">
       <c r="A141">
-        <v>15063</v>
+        <v>15265</v>
       </c>
       <c r="B141">
-        <v>1.1799999999999999</v>
+        <v>1.6200000000000001</v>
       </c>
       <c r="C141">
-        <v>-1</v>
+        <v>44</v>
       </c>
     </row>
     <row r="142">
       <c r="A142">
-        <v>15164</v>
+        <v>15365</v>
       </c>
       <c r="B142">
-        <v>1.03</v>
+        <v>1.6200000000000001</v>
       </c>
       <c r="C142">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="143">
       <c r="A143">
-        <v>15265</v>
+        <v>15467</v>
       </c>
       <c r="B143">
-        <v>0.96999999999999997</v>
+        <v>1.6399999999999999</v>
       </c>
       <c r="C143">
-        <v>-1</v>
+        <v>55</v>
       </c>
     </row>
     <row r="144">
       <c r="A144">
-        <v>15365</v>
+        <v>15567</v>
       </c>
       <c r="B144">
-        <v>0.82999999999999996</v>
+        <v>1.6499999999999999</v>
       </c>
       <c r="C144">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="145">
       <c r="A145">
-        <v>15467</v>
+        <v>15668</v>
       </c>
       <c r="B145">
-        <v>0.79000000000000004</v>
+        <v>1.6200000000000001</v>
       </c>
       <c r="C145">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="146">
       <c r="A146">
-        <v>15568</v>
+        <v>15770</v>
       </c>
       <c r="B146">
-        <v>1.1000000000000001</v>
+        <v>1.5900000000000001</v>
       </c>
       <c r="C146">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="147">
       <c r="A147">
-        <v>15668</v>
+        <v>15870</v>
       </c>
       <c r="B147">
-        <v>1.3500000000000001</v>
+        <v>1.6000000000000001</v>
       </c>
       <c r="C147">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="148">
       <c r="A148">
-        <v>15770</v>
+        <v>15971</v>
       </c>
       <c r="B148">
-        <v>1.4399999999999999</v>
+        <v>1.6699999999999999</v>
       </c>
       <c r="C148">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="149">
       <c r="A149">
-        <v>15870</v>
+        <v>16072</v>
       </c>
       <c r="B149">
-        <v>1.5</v>
+        <v>1.6499999999999999</v>
       </c>
       <c r="C149">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="150">
       <c r="A150">
-        <v>15971</v>
+        <v>16173</v>
       </c>
       <c r="B150">
-        <v>1.53</v>
+        <v>1.6499999999999999</v>
       </c>
       <c r="C150">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="151">
       <c r="A151">
-        <v>16072</v>
+        <v>16273</v>
       </c>
       <c r="B151">
-        <v>1.55</v>
+        <v>1.6499999999999999</v>
       </c>
       <c r="C151">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="152">
       <c r="A152">
-        <v>16173</v>
+        <v>16393</v>
       </c>
       <c r="B152">
-        <v>1.4099999999999999</v>
+        <v>1.55</v>
       </c>
       <c r="C152">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="153">
       <c r="A153">
-        <v>16275</v>
+        <v>16494</v>
       </c>
       <c r="B153">
-        <v>1.05</v>
+        <v>1.4299999999999999</v>
       </c>
       <c r="C153">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="154">
       <c r="A154">
-        <v>16393</v>
+        <v>16595</v>
       </c>
       <c r="B154">
-        <v>0.90000000000000002</v>
+        <v>1.5700000000000001</v>
       </c>
       <c r="C154">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="155">
       <c r="A155">
-        <v>16495</v>
+        <v>16696</v>
       </c>
       <c r="B155">
-        <v>0.55000000000000004</v>
+        <v>1.6100000000000001</v>
       </c>
       <c r="C155">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="156">
       <c r="A156">
-        <v>16595</v>
+        <v>16797</v>
       </c>
       <c r="B156">
-        <v>0.53000000000000003</v>
+        <v>1.6499999999999999</v>
       </c>
       <c r="C156">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="157">
       <c r="A157">
-        <v>16696</v>
+        <v>16898</v>
       </c>
       <c r="B157">
-        <v>0.66000000000000003</v>
+        <v>1.6100000000000001</v>
       </c>
       <c r="C157">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="158">
       <c r="A158">
-        <v>16797</v>
+        <v>16998</v>
       </c>
       <c r="B158">
-        <v>0.76000000000000001</v>
+        <v>1.6000000000000001</v>
       </c>
       <c r="C158">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="159">
       <c r="A159">
-        <v>16898</v>
+        <v>17100</v>
       </c>
       <c r="B159">
-        <v>0.83999999999999997</v>
+        <v>1.5800000000000001</v>
       </c>
       <c r="C159">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="160">
       <c r="A160">
-        <v>16999</v>
+        <v>17201</v>
       </c>
       <c r="B160">
-        <v>0.78000000000000003</v>
+        <v>1.5900000000000001</v>
       </c>
       <c r="C160">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="161">
       <c r="A161">
-        <v>17100</v>
+        <v>17302</v>
       </c>
       <c r="B161">
-        <v>0.66000000000000003</v>
+        <v>1.6399999999999999</v>
       </c>
       <c r="C161">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="162">
       <c r="A162">
-        <v>17201</v>
+        <v>17403</v>
       </c>
       <c r="B162">
-        <v>0.68000000000000005</v>
+        <v>1.6399999999999999</v>
       </c>
       <c r="C162">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="163">
       <c r="A163">
-        <v>17302</v>
+        <v>17503</v>
       </c>
       <c r="B163">
-        <v>0.75</v>
+        <v>1.6799999999999999</v>
       </c>
       <c r="C163">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="164">
       <c r="A164">
-        <v>17403</v>
+        <v>17605</v>
       </c>
       <c r="B164">
-        <v>0.78000000000000003</v>
+        <v>1.74</v>
       </c>
       <c r="C164">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="165">
       <c r="A165">
-        <v>17503</v>
+        <v>17705</v>
       </c>
       <c r="B165">
-        <v>0.76000000000000001</v>
+        <v>1.74</v>
       </c>
       <c r="C165">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="166">
       <c r="A166">
-        <v>17605</v>
+        <v>17806</v>
       </c>
       <c r="B166">
-        <v>0.5</v>
+        <v>1.6899999999999999</v>
       </c>
       <c r="C166">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="167">
       <c r="A167">
-        <v>17705</v>
+        <v>17908</v>
       </c>
       <c r="B167">
-        <v>0.63</v>
+        <v>1.6499999999999999</v>
       </c>
       <c r="C167">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="168">
+      <c r="A168">
+        <v>18008</v>
+      </c>
       <c r="B168">
-        <v>0.46999999999999997</v>
+        <v>1.5700000000000001</v>
       </c>
       <c r="C168">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="169">
       <c r="A169">
-        <v>18008</v>
+        <v>18109</v>
       </c>
       <c r="B169">
-        <v>0.089999999999999997</v>
+        <v>1.5800000000000001</v>
       </c>
       <c r="C169">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="170">
       <c r="A170">
-        <v>18110</v>
+        <v>18430</v>
       </c>
       <c r="B170">
-        <v>0</v>
+        <v>2.0299999999999998</v>
       </c>
       <c r="C170">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="171">
       <c r="A171">
-        <v>18430</v>
+        <v>18531</v>
       </c>
       <c r="B171">
-        <v>0.23000000000000001</v>
+        <v>2.02</v>
       </c>
       <c r="C171">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="172">
       <c r="A172">
-        <v>18531</v>
+        <v>18633</v>
       </c>
       <c r="B172">
-        <v>0.42999999999999999</v>
+        <v>2.0299999999999998</v>
       </c>
       <c r="C172">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="173">
       <c r="A173">
-        <v>18632</v>
+        <v>18733</v>
       </c>
       <c r="B173">
-        <v>0.52000000000000002</v>
+        <v>1.99</v>
       </c>
       <c r="C173">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="174">
       <c r="A174">
-        <v>18733</v>
+        <v>18834</v>
       </c>
       <c r="B174">
-        <v>0.47999999999999998</v>
+        <v>1.96</v>
       </c>
       <c r="C174">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="175">
       <c r="A175">
-        <v>18834</v>
+        <v>18935</v>
       </c>
       <c r="B175">
-        <v>0.57999999999999996</v>
+        <v>1.9099999999999999</v>
       </c>
       <c r="C175">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="176">
       <c r="A176">
-        <v>18935</v>
+        <v>19036</v>
       </c>
       <c r="B176">
-        <v>0.73999999999999999</v>
+        <v>1.9099999999999999</v>
       </c>
       <c r="C176">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="177">
       <c r="A177">
-        <v>19035</v>
+        <v>19138</v>
       </c>
       <c r="B177">
-        <v>0.87</v>
+        <v>1.8700000000000001</v>
       </c>
       <c r="C177">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="178">
       <c r="A178">
-        <v>19137</v>
+        <v>19238</v>
       </c>
       <c r="B178">
-        <v>1.02</v>
+        <v>1.8200000000000001</v>
       </c>
       <c r="C178">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="179">
       <c r="A179">
-        <v>19237</v>
+        <v>19339</v>
       </c>
       <c r="B179">
-        <v>1.1299999999999999</v>
+        <v>1.71</v>
       </c>
       <c r="C179">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="180">
       <c r="A180">
-        <v>19338</v>
+        <v>19641</v>
       </c>
       <c r="B180">
-        <v>1.26</v>
+        <v>1.6599999999999999</v>
       </c>
       <c r="C180">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="181">
       <c r="A181">
-        <v>19440</v>
+        <v>19743</v>
       </c>
       <c r="B181">
-        <v>1.3600000000000001</v>
+        <v>1.6100000000000001</v>
       </c>
       <c r="C181">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="182">
       <c r="A182">
-        <v>19540</v>
+        <v>19844</v>
       </c>
       <c r="B182">
-        <v>1.3400000000000001</v>
+        <v>1.55</v>
       </c>
       <c r="C182">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="183">
       <c r="A183">
-        <v>19843</v>
+        <v>19944</v>
       </c>
       <c r="B183">
-        <v>1.0600000000000001</v>
+        <v>1.5</v>
       </c>
       <c r="C183">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="184">
       <c r="A184">
-        <v>19944</v>
+        <v>20046</v>
       </c>
       <c r="B184">
-        <v>0.75</v>
+        <v>1.45</v>
       </c>
       <c r="C184">
-        <v>-1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="185">
       <c r="A185">
-        <v>20045</v>
+        <v>20146</v>
       </c>
       <c r="B185">
-        <v>0.81999999999999995</v>
+        <v>1.49</v>
       </c>
       <c r="C185">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="186">
       <c r="A186">
-        <v>20146</v>
+        <v>20248</v>
       </c>
       <c r="B186">
-        <v>0.93000000000000005</v>
+        <v>1.49</v>
       </c>
       <c r="C186">
-        <v>-1</v>
+        <v>53</v>
       </c>
     </row>
     <row r="187">
       <c r="A187">
-        <v>20247</v>
+        <v>20468</v>
       </c>
       <c r="B187">
-        <v>1.01</v>
+        <v>1.95</v>
       </c>
       <c r="C187">
-        <v>-1</v>
+        <v>51</v>
       </c>
     </row>
     <row r="188">
       <c r="A188">
-        <v>20348</v>
+        <v>20569</v>
       </c>
       <c r="B188">
-        <v>1.1299999999999999</v>
+        <v>1.73</v>
       </c>
       <c r="C188">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="189">
       <c r="A189">
-        <v>20467</v>
+        <v>20669</v>
       </c>
       <c r="B189">
-        <v>1.1899999999999999</v>
+        <v>1.7</v>
       </c>
       <c r="C189">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="190">
       <c r="A190">
-        <v>20568</v>
+        <v>20771</v>
       </c>
       <c r="B190">
-        <v>1.24</v>
+        <v>1.6499999999999999</v>
       </c>
       <c r="C190">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="191">
       <c r="A191">
-        <v>20669</v>
+        <v>20871</v>
       </c>
       <c r="B191">
-        <v>1.3100000000000001</v>
+        <v>1.5700000000000001</v>
       </c>
       <c r="C191">
-        <v>-1</v>
+        <v>48</v>
       </c>
     </row>
     <row r="192">
       <c r="A192">
-        <v>20972</v>
+        <v>20973</v>
       </c>
       <c r="B192">
-        <v>1.28</v>
+        <v>1.3600000000000001</v>
       </c>
       <c r="C192">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="193">
       <c r="A193">
-        <v>21072</v>
+        <v>21074</v>
       </c>
       <c r="B193">
-        <v>1.3200000000000001</v>
+        <v>1.24</v>
       </c>
       <c r="C193">
-        <v>-1</v>
+        <v>51</v>
       </c>
     </row>
     <row r="194">
       <c r="A194">
-        <v>21173</v>
+        <v>21174</v>
       </c>
       <c r="B194">
-        <v>1.3500000000000001</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="C194">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="195">
       <c r="A195">
-        <v>21275</v>
+        <v>21276</v>
       </c>
       <c r="B195">
-        <v>1.3500000000000001</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="C195">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="196">
       <c r="A196">
-        <v>21375</v>
+        <v>21477</v>
       </c>
       <c r="B196">
-        <v>1.3500000000000001</v>
+        <v>0.98999999999999999</v>
       </c>
       <c r="C196">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="197">
       <c r="A197">
-        <v>21477</v>
+        <v>21578</v>
       </c>
       <c r="B197">
-        <v>1.3</v>
+        <v>0.93000000000000005</v>
       </c>
       <c r="C197">
-        <v>-1</v>
+        <v>48</v>
       </c>
     </row>
     <row r="198">
       <c r="A198">
-        <v>21577</v>
+        <v>21679</v>
       </c>
       <c r="B198">
-        <v>1.29</v>
+        <v>0.92000000000000004</v>
       </c>
       <c r="C198">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="199">
       <c r="A199">
-        <v>21678</v>
+        <v>21780</v>
       </c>
       <c r="B199">
-        <v>1.3400000000000001</v>
+        <v>0.90000000000000002</v>
       </c>
       <c r="C199">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="200">
       <c r="A200">
-        <v>21981</v>
+        <v>21881</v>
       </c>
       <c r="B200">
-        <v>1.3700000000000001</v>
+        <v>0.90000000000000002</v>
       </c>
       <c r="C200">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="201">
       <c r="A201">
-        <v>22082</v>
+        <v>21982</v>
       </c>
       <c r="B201">
-        <v>1.3999999999999999</v>
+        <v>0.87</v>
       </c>
       <c r="C201">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="202">
       <c r="A202">
-        <v>22183</v>
+        <v>22083</v>
       </c>
       <c r="B202">
-        <v>1.3999999999999999</v>
+        <v>0.79000000000000004</v>
       </c>
       <c r="C202">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="203">
       <c r="A203">
-        <v>22283</v>
+        <v>22284</v>
       </c>
       <c r="B203">
-        <v>1.4399999999999999</v>
+        <v>0.72999999999999998</v>
       </c>
       <c r="C203">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="204">
       <c r="A204">
-        <v>22385</v>
+        <v>22386</v>
       </c>
       <c r="B204">
-        <v>1.46</v>
+        <v>0.77000000000000002</v>
       </c>
       <c r="C204">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="205">
@@ -2418,76 +2533,76 @@
         <v>22504</v>
       </c>
       <c r="B205">
-        <v>1.4399999999999999</v>
+        <v>1.24</v>
       </c>
       <c r="C205">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="206">
       <c r="A206">
-        <v>22605</v>
+        <v>22606</v>
       </c>
       <c r="B206">
-        <v>1.4299999999999999</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="C206">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="207">
       <c r="A207">
-        <v>22705</v>
+        <v>22707</v>
       </c>
       <c r="B207">
-        <v>1.47</v>
+        <v>1.24</v>
       </c>
       <c r="C207">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="208">
       <c r="A208">
-        <v>22807</v>
+        <v>22808</v>
       </c>
       <c r="B208">
-        <v>1.47</v>
+        <v>1.78</v>
       </c>
       <c r="C208">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="209">
       <c r="A209">
-        <v>22908</v>
+        <v>22909</v>
       </c>
       <c r="B209">
-        <v>1.49</v>
+        <v>1.8400000000000001</v>
       </c>
       <c r="C209">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="210">
       <c r="A210">
-        <v>23008</v>
+        <v>23212</v>
       </c>
       <c r="B210">
-        <v>1.52</v>
+        <v>2.1000000000000001</v>
       </c>
       <c r="C210">
-        <v>-1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="211">
       <c r="A211">
-        <v>23110</v>
+        <v>23312</v>
       </c>
       <c r="B211">
-        <v>1.55</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="C211">
-        <v>-1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="212">

</xml_diff>